<commit_message>
Bukatuta Aurkezpena eta txostena
</commit_message>
<xml_diff>
--- a/0.1- PLANIFIKAZIOA/TSB EGUNEROKOA.xlsx
+++ b/0.1- PLANIFIKAZIOA/TSB EGUNEROKOA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elect\OneDrive\Escritorio\ERRONKA-TSB-RETURNS\0.1- PLANIFIKAZIOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3850E172-D8D9-45D1-83A9-1547648337D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44759AD4-ED14-469B-A893-530990EA2616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="82">
   <si>
     <t>ENTREGA</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>TALDEA: Erronkaren aurkezpena egin</t>
+  </si>
+  <si>
+    <t>INTERFAZ: Aplikazioaren dokumentazioa atera</t>
   </si>
 </sst>
 </file>
@@ -1010,41 +1013,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1064,6 +1032,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1094,6 +1071,32 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1571,8 +1574,8 @@
   </sheetPr>
   <dimension ref="A1:Y854"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1586,18 +1589,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="34.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
       <c r="G1" s="10"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="49"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1615,18 +1618,18 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="34.5" x14ac:dyDescent="0.95">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="35"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1644,16 +1647,16 @@
       <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:25" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1698,17 +1701,17 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" ht="29.25" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="4"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1727,21 +1730,21 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70" t="s">
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="57"/>
       <c r="J6" s="33" t="s">
         <v>17</v>
       </c>
@@ -1762,21 +1765,21 @@
       <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="43" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="43" t="s">
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="30" t="s">
         <v>21</v>
       </c>
@@ -1797,19 +1800,19 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="46" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="70"/>
       <c r="J8" s="31" t="s">
         <v>23</v>
       </c>
@@ -1830,19 +1833,19 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="34" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="36"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="32" t="s">
         <v>25</v>
       </c>
@@ -1869,11 +1872,11 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="8"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1919,30 +1922,30 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="19.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="61" t="s">
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="66" t="s">
+      <c r="H12" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K12" s="1"/>
@@ -1962,9 +1965,9 @@
       <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="1:25" ht="20.25" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="60"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="9" t="s">
         <v>4</v>
       </c>
@@ -1974,10 +1977,10 @@
       <c r="F13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="55"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2009,7 +2012,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
       <c r="H14" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>28</v>
@@ -2298,11 +2301,11 @@
         <v>47</v>
       </c>
       <c r="C22" s="18"/>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="E22" s="18"/>
-      <c r="F22" s="17" t="s">
-        <v>32</v>
-      </c>
+      <c r="F22" s="17"/>
       <c r="G22" s="18"/>
       <c r="H22" s="17" t="s">
         <v>32</v>
@@ -2335,11 +2338,11 @@
         <v>42</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="17" t="s">
-        <v>29</v>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17" t="s">
+        <v>31</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="17"/>
       <c r="G23" s="18"/>
       <c r="H23" s="17" t="s">
         <v>31</v>
@@ -2409,11 +2412,11 @@
         <v>44</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="17"/>
+      <c r="D25" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="E25" s="18"/>
-      <c r="F25" s="17" t="s">
-        <v>32</v>
-      </c>
+      <c r="F25" s="17"/>
       <c r="G25" s="18"/>
       <c r="H25" s="17" t="s">
         <v>32</v>
@@ -2483,14 +2486,14 @@
         <v>46</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="17" t="s">
-        <v>29</v>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17" t="s">
+        <v>31</v>
       </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="17"/>
       <c r="G27" s="18"/>
       <c r="H27" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>28</v>
@@ -2712,7 +2715,7 @@
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
       <c r="H33" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>28</v>
@@ -2853,14 +2856,14 @@
         <v>56</v>
       </c>
       <c r="C37" s="24"/>
-      <c r="D37" s="23" t="s">
-        <v>29</v>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="23" t="s">
+        <v>31</v>
       </c>
-      <c r="E37" s="24"/>
-      <c r="F37" s="23"/>
       <c r="G37" s="24"/>
       <c r="H37" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>28</v>
@@ -2927,14 +2930,14 @@
         <v>58</v>
       </c>
       <c r="C39" s="24"/>
-      <c r="D39" s="23" t="s">
-        <v>29</v>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="23" t="s">
+        <v>31</v>
       </c>
-      <c r="E39" s="24"/>
-      <c r="F39" s="23"/>
       <c r="G39" s="24"/>
       <c r="H39" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>28</v>
@@ -3038,14 +3041,14 @@
         <v>63</v>
       </c>
       <c r="C42" s="24"/>
-      <c r="D42" s="23" t="s">
-        <v>29</v>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="23" t="s">
+        <v>31</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="23"/>
       <c r="G42" s="24"/>
       <c r="H42" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>28</v>
@@ -3156,7 +3159,7 @@
       <c r="F45" s="23"/>
       <c r="G45" s="24"/>
       <c r="H45" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>28</v>
@@ -3482,14 +3485,14 @@
         <v>77</v>
       </c>
       <c r="C54" s="24"/>
-      <c r="D54" s="23" t="s">
-        <v>29</v>
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23" t="s">
+        <v>31</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="23"/>
       <c r="G54" s="24"/>
       <c r="H54" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>28</v>
@@ -3556,11 +3559,11 @@
         <v>80</v>
       </c>
       <c r="C56" s="24"/>
-      <c r="D56" s="23" t="s">
-        <v>29</v>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="23" t="s">
+        <v>31</v>
       </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="23"/>
       <c r="G56" s="24"/>
       <c r="H56" s="23" t="s">
         <v>31</v>
@@ -3586,16 +3589,24 @@
       <c r="Y56" s="1"/>
     </row>
     <row r="57" spans="1:25" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="22"/>
-      <c r="B57" s="29"/>
+      <c r="A57" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>81</v>
+      </c>
       <c r="C57" s="24"/>
       <c r="D57" s="23"/>
       <c r="E57" s="24"/>
-      <c r="F57" s="23"/>
+      <c r="F57" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="G57" s="24"/>
-      <c r="H57" s="23"/>
+      <c r="H57" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="I57" s="8" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="J57" s="24"/>
       <c r="K57" s="1"/>
@@ -25145,6 +25156,16 @@
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
   <mergeCells count="26">
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="J12:J13"/>
@@ -25161,16 +25182,6 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="B14:B60">
     <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="ENPRESA:">
@@ -25200,7 +25211,7 @@
       <formula>NOT(ISERROR(SEARCH("TSB",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F60 H14:H60">
+  <conditionalFormatting sqref="H14:H60 F14:F60">
     <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="LANDER">
       <formula>NOT(ISERROR(SEARCH("LANDER",F14)))</formula>
     </cfRule>

</xml_diff>